<commit_message>
adding combobox for selecting the sectoral unions
</commit_message>
<xml_diff>
--- a/ApplicationCode/subscriberlist.xlsx
+++ b/ApplicationCode/subscriberlist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1197,10 +1197,41 @@
           <t>12345678</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
           <t>Option 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>zdz</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>4RE</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>الماشية</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing the error messages
</commit_message>
<xml_diff>
--- a/ApplicationCode/subscriberlist.xlsx
+++ b/ApplicationCode/subscriberlist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1235,6 +1235,230 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ERE</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>FS</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>14000000</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>98625905</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>GRG</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>السقوي</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>RR</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>RR</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>22334455</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>EE</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>الصيد بالأضواء</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>jjj</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>jjj</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>TGFF</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>الماشية</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>UUUU</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>YYYY</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>12335511</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>11223344</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>HHH</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>الصيد الساحلي</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ggf</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>32323323</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>السقوي</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>RRR</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CGG</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>rrrr</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>الزياتين</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>433</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>DDD</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>12121212</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>12121212</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>FFF</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>الصيد بالأضواء</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing the data base after adding the second combobox
</commit_message>
<xml_diff>
--- a/ApplicationCode/subscriberlist.xlsx
+++ b/ApplicationCode/subscriberlist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1459,6 +1459,43 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>EZEZ</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>44331122</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>11223344</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>fdfdd</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>الماشية</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>الأبقار</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing the search function after adding the combobox
</commit_message>
<xml_diff>
--- a/ApplicationCode/subscriberlist.xlsx
+++ b/ApplicationCode/subscriberlist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1496,6 +1496,80 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>EEEF</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>FFDF</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>11223344</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>11223344</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>efe</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>الماشية</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>الأبقار</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>TJT</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>FDDF</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>11223344</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>11223344</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>DDZ</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>الماشية</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>الأغنام</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adding the automatically creation of the .xlsx sheet if it does not exist
</commit_message>
<xml_diff>
--- a/ApplicationCode/subscriberlist.xlsx
+++ b/ApplicationCode/subscriberlist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:G3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,136 +421,35 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="0">
-      <c r="A0" t="inlineStr">
-        <is>
-          <t>naoures</t>
-        </is>
-      </c>
-      <c r="B0" t="inlineStr">
-        <is>
-          <t>bzeouich</t>
-        </is>
-      </c>
-      <c r="C0" t="inlineStr">
-        <is>
-          <t>14034110</t>
-        </is>
-      </c>
-      <c r="D0" t="inlineStr">
-        <is>
-          <t>97944447</t>
-        </is>
-      </c>
-      <c r="E0" t="inlineStr">
-        <is>
-          <t>MOKNINE</t>
-        </is>
-      </c>
-      <c r="F0" t="inlineStr">
-        <is>
-          <t>الزياتين</t>
-        </is>
-      </c>
-    </row>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>mohamed</t>
+          <t>ve</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>bzeouich</t>
+          <t>dds</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>04040404</t>
+          <t>12345678</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>97487999</t>
+          <t>12345678</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>MOKNINE</t>
+          <t>GN</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>السقوي</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hayet </t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>gannouni</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>03030303</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>90909090</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ksar hlel</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>الماشية</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>الأغنام</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>heyet</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ganouni</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>14141414</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>90999099</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ksar hlel</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>الصيد بالأضواء</t>
+          <t>النحل</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixe some bugs in the deletion functions
</commit_message>
<xml_diff>
--- a/ApplicationCode/subscriberlist.xlsx
+++ b/ApplicationCode/subscriberlist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A0:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,52 +421,94 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="0">
+      <c r="A0" t="inlineStr">
+        <is>
+          <t>ZZ</t>
+        </is>
+      </c>
+      <c r="B0" t="inlineStr">
+        <is>
+          <t>RR</t>
+        </is>
+      </c>
+      <c r="C0" t="inlineStr">
+        <is>
+          <t>11223344</t>
+        </is>
+      </c>
+      <c r="D0" t="inlineStr">
+        <is>
+          <t>11223344</t>
+        </is>
+      </c>
+      <c r="E0" t="inlineStr">
+        <is>
+          <t>FFG</t>
+        </is>
+      </c>
+      <c r="F0" t="inlineStr">
+        <is>
+          <t>الماشية</t>
+        </is>
+      </c>
+      <c r="G0" t="inlineStr">
+        <is>
+          <t>الأبقار</t>
+        </is>
+      </c>
+    </row>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">: اسم </t>
+          <t>mohamed</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t xml:space="preserve">: اللقب </t>
+          <t>bzeouich</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> : رقم بطاقة الهوية الوطنية </t>
+          <t>04040404</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t xml:space="preserve">: رقم الهاتف </t>
+          <t>97487999</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> : المنطقة </t>
+          <t>sousine</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> :النقابات القطاعية</t>
+          <t>الماشية</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>الأبقار</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ge</t>
+          <t>mkezlmkfz</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>errg</t>
+          <t>jfzbjb</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>44332211</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -476,49 +518,140 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>TYHT</t>
+          <t>sousine</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>الزياتين</t>
+          <t>السقوي</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ZZ</t>
+          <t>lvkjlkj</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>ekjej</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11223344</t>
+          <t>99887766</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>11223344</t>
+          <t>99119911</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>FFG</t>
+          <t>ksar hlel</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>الصيد الساحلي</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>elkl</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>;efrne</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>33445566</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>33445566</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>moknine</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>الماشية</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>الأبقار</t>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GRLK</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>LKLGE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>44556677</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>44556677</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>KJEFL</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>الصيد بالأضواء</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>evf</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>v;:</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>55667788</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>55667788</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>EG?ELMK</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>الصيد الساحلي</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
creating an standalone executable file
</commit_message>
<xml_diff>
--- a/ApplicationCode/subscriberlist.xlsx
+++ b/ApplicationCode/subscriberlist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:G6"/>
+  <dimension ref="A0:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,128 +530,64 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>lvkjlkj</t>
+          <t>elkl</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ekjej</t>
+          <t>;efrne</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>99887766</t>
+          <t>33445566</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>99119911</t>
+          <t>33445566</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ksar hlel</t>
+          <t>moknine</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>الصيد الساحلي</t>
+          <t>الماشية</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>elkl</t>
+          <t>naoures</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>;efrne</t>
+          <t>bzeouich</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>33445566</t>
+          <t>14034112</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>33445566</t>
+          <t>97944447</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>moknine</t>
+          <t>MOKNINE</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>الماشية</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>GRLK</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>LKLGE</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>44556677</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>44556677</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>KJEFL</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>الصيد بالأضواء</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>evf</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>v;:</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>55667788</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>55667788</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>EG?ELMK</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>الصيد الساحلي</t>
+          <t>النحل</t>
         </is>
       </c>
     </row>

</xml_diff>